<commit_message>
tinker with the main file, finalized is for rollback
</commit_message>
<xml_diff>
--- a/exam hall try1/2ND YEAR.xlsx
+++ b/exam hall try1/2ND YEAR.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -35,6 +35,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -68,10 +74,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -393,112 +399,112 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2">
         <v>22000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2">
         <v>22001</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2">
         <v>22002</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2">
         <v>22003</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2">
         <v>22004</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2">
         <v>22005</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2">
         <v>22006</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2">
         <v>22007</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="2">
         <v>22008</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="2">
         <v>22009</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2">
         <v>22010</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="2">
         <v>22011</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="2">
         <v>22012</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="2">
         <v>22013</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="2">
         <v>22014</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="2">
         <v>22015</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="2">
         <v>22016</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="2">
         <v>22017</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="2">
         <v>22018</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="2">
         <v>22019</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="2">
         <v>22020</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="2">
         <v>22021</v>
       </c>

</xml_diff>